<commit_message>
Update Paypal Payment Details Today 16Sep24.xlsx
Money is on its way to my bank. ETA 1st Oct 24.
</commit_message>
<xml_diff>
--- a/z Money/Paypal Payment Details Today 16Sep24.xlsx
+++ b/z Money/Paypal Payment Details Today 16Sep24.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -60,9 +60,6 @@
     <t>26/09/24, 11:08 p.m.</t>
   </si>
   <si>
-    <t>Completedtooltip1</t>
-  </si>
-  <si>
     <t>Dollars</t>
   </si>
   <si>
@@ -73,13 +70,44 @@
   </si>
   <si>
     <t>Net %</t>
+  </si>
+  <si>
+    <t>Trasnfered from PayPal</t>
+  </si>
+  <si>
+    <t>INVOICE#001</t>
+  </si>
+  <si>
+    <t>INVOICE#002</t>
+  </si>
+  <si>
+    <t>INVOICE#003</t>
+  </si>
+  <si>
+    <t>Got in Bank</t>
+  </si>
+  <si>
+    <t>28/09/24, 04:35 a.m.</t>
+  </si>
+  <si>
+    <t>$1 = ₹80.66</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>Overall%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="165" formatCode="_ [$₹-4009]\ * #,##0.00_ ;_ [$₹-4009]\ * \-#,##0.00_ ;_ [$₹-4009]\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +119,30 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -148,10 +200,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -159,6 +210,18 @@
     <xf numFmtId="4" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,10 +524,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,16 +535,19 @@
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.28515625" customWidth="1"/>
     <col min="10" max="11" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,7 +563,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -506,15 +572,15 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
+      <c r="I1" s="2"/>
       <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -525,31 +591,31 @@
         <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2" s="11">
         <v>500</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="12">
         <v>26.31</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="11">
         <v>473.69</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="6">
+      <c r="I2" s="3"/>
+      <c r="J2" s="5">
         <f>F2/E2*100</f>
         <v>5.2620000000000005</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="5">
         <f>G2/E2*100</f>
         <v>94.738</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -560,31 +626,31 @@
         <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3" s="11">
         <v>750</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="12">
         <v>39.29</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="11">
         <v>710.71</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="4"/>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:K6" si="0">F3/E3*100</f>
+      <c r="I3" s="3"/>
+      <c r="J3" s="5">
+        <f t="shared" ref="J3:J6" si="0">F3/E3*100</f>
         <v>5.2386666666666661</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <f t="shared" ref="K3:K6" si="1">G3/E3*100</f>
         <v>94.76133333333334</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -595,80 +661,223 @@
         <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="2">
+        <v>21</v>
+      </c>
+      <c r="E4" s="11">
         <v>1750</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="12">
         <v>91.21</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="11">
         <v>1658.79</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="6">
+      <c r="I4" s="3"/>
+      <c r="J4" s="5">
         <f t="shared" si="0"/>
         <v>5.2119999999999997</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <f t="shared" si="1"/>
         <v>94.787999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E5" s="7">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E5" s="13">
         <f>SUM(E2:E4)</f>
         <v>3000</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="14">
         <f t="shared" ref="F5:G5" si="2">SUM(F2:F4)</f>
         <v>156.81</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="13">
         <f t="shared" si="2"/>
         <v>2843.19</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="5"/>
-      <c r="J5" s="9">
+      <c r="H5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="8">
         <f t="shared" si="0"/>
         <v>5.2270000000000003</v>
       </c>
-      <c r="K5" s="9">
+      <c r="K5" s="8">
         <f t="shared" si="1"/>
         <v>94.77300000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E6" s="7">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E6" s="15">
         <f>E5*83.64</f>
         <v>250920</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="16">
         <f t="shared" ref="F6:G6" si="3">F5*83.64</f>
         <v>13115.588400000001</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="18">
         <f t="shared" si="3"/>
         <v>237804.41159999999</v>
       </c>
-      <c r="H6" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="9">
+      <c r="H6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="3"/>
+      <c r="J6" s="8">
         <f t="shared" si="0"/>
         <v>5.2270000000000003</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="8">
         <f t="shared" si="1"/>
         <v>94.772999999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E8" s="13">
+        <f>G8/83.64</f>
+        <v>2741.9154710664752</v>
+      </c>
+      <c r="F8" s="14">
+        <f>G5-E8</f>
+        <v>101.27452893352483</v>
+      </c>
+      <c r="G8" s="15">
+        <v>229333.81</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" s="8">
+        <f>G10/E5*100</f>
+        <v>91.397182368882511</v>
+      </c>
+      <c r="N8" s="11">
+        <f>E5*M8%</f>
+        <v>2741.9154710664752</v>
+      </c>
+      <c r="O8" s="19">
+        <f>E6*M8%</f>
+        <v>229333.81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M9" s="8">
+        <f>(F10+F5)/E5*100</f>
+        <v>8.6028176311174942</v>
+      </c>
+      <c r="N9" s="11">
+        <f>E5*M9%</f>
+        <v>258.08452893352484</v>
+      </c>
+      <c r="O9" s="20">
+        <f>E6*M9%</f>
+        <v>21586.190000000017</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="13">
+        <v>2843.19</v>
+      </c>
+      <c r="F10" s="14">
+        <f>E10-G10</f>
+        <v>101.27452893352483</v>
+      </c>
+      <c r="G10" s="13">
+        <v>2741.9154710664752</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" ref="J10" si="4">F10/E10*100</f>
+        <v>3.5620035570441946</v>
+      </c>
+      <c r="K10" s="8">
+        <f t="shared" ref="K10" si="5">G10/E10*100</f>
+        <v>96.437996442955807</v>
+      </c>
+      <c r="N10" s="13">
+        <f>SUM(N8:N9)</f>
+        <v>3000</v>
+      </c>
+      <c r="O10" s="15">
+        <f>SUM(O8:O9)</f>
+        <v>250920</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="15">
+        <f>E10*83.64</f>
+        <v>237804.41159999999</v>
+      </c>
+      <c r="F11" s="16">
+        <f t="shared" ref="F11:G11" si="6">F10*83.64</f>
+        <v>8470.6016000000163</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="6"/>
+        <v>229333.81</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" ref="J11" si="7">F11/E11*100</f>
+        <v>3.5620035570441946</v>
+      </c>
+      <c r="K11" s="8">
+        <f t="shared" ref="K11" si="8">G11/E11*100</f>
+        <v>96.437996442955821</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12" s="10"/>
+      <c r="N12" s="7" t="b">
+        <f>N9=F5+F10</f>
+        <v>1</v>
+      </c>
+      <c r="O12" s="7" t="b">
+        <f>O9=F6+F11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H13" s="7" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>